<commit_message>
Removed all the pT values less than 1 GeV.
</commit_message>
<xml_diff>
--- a/database/AN_ep/expdata/1004.xlsx
+++ b/database/AN_ep/expdata/1004.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="14">
   <si>
     <t xml:space="preserve">xF</t>
   </si>
@@ -171,7 +171,7 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
+      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -213,7 +213,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>0.001</v>
@@ -245,7 +245,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>0.001</v>
@@ -277,7 +277,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>0.001</v>
@@ -309,7 +309,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>0.001</v>
@@ -341,7 +341,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>0.001</v>
@@ -373,7 +373,7 @@
         <v>0</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>0.001</v>
@@ -405,7 +405,7 @@
         <v>0</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>0.001</v>
@@ -437,7 +437,7 @@
         <v>0</v>
       </c>
       <c r="B9" s="2" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>0.001</v>
@@ -469,7 +469,7 @@
         <v>0</v>
       </c>
       <c r="B10" s="2" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C10" s="1" t="n">
         <v>0.001</v>
@@ -501,7 +501,7 @@
         <v>0</v>
       </c>
       <c r="B11" s="2" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C11" s="1" t="n">
         <v>0.001</v>
@@ -533,7 +533,7 @@
         <v>0</v>
       </c>
       <c r="B12" s="2" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C12" s="1" t="n">
         <v>0.001</v>
@@ -565,7 +565,7 @@
         <v>0</v>
       </c>
       <c r="B13" s="2" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C13" s="1" t="n">
         <v>0.001</v>
@@ -597,7 +597,7 @@
         <v>0</v>
       </c>
       <c r="B14" s="2" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C14" s="1" t="n">
         <v>0.001</v>
@@ -629,7 +629,7 @@
         <v>0</v>
       </c>
       <c r="B15" s="2" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C15" s="1" t="n">
         <v>0.001</v>
@@ -661,7 +661,7 @@
         <v>0</v>
       </c>
       <c r="B16" s="2" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C16" s="1" t="n">
         <v>0.001</v>
@@ -693,7 +693,7 @@
         <v>0</v>
       </c>
       <c r="B17" s="2" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C17" s="1" t="n">
         <v>0.001</v>
@@ -721,36 +721,16 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="B18" s="2" t="n">
-        <v>16</v>
-      </c>
-      <c r="C18" s="1" t="n">
-        <v>0.001</v>
-      </c>
-      <c r="D18" s="1" t="n">
-        <v>0.001</v>
-      </c>
-      <c r="E18" s="1" t="n">
-        <v>0.001</v>
-      </c>
-      <c r="F18" s="2" t="n">
-        <v>63</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
xF=0.6 instead of 0.
</commit_message>
<xml_diff>
--- a/database/AN_ep/expdata/1004.xlsx
+++ b/database/AN_ep/expdata/1004.xlsx
@@ -171,7 +171,7 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -210,7 +210,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="B2" s="2" t="n">
         <v>1</v>
@@ -242,7 +242,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="n">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>2</v>
@@ -274,7 +274,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="n">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>3</v>
@@ -306,7 +306,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="n">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>4</v>
@@ -338,7 +338,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="n">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="B6" s="2" t="n">
         <v>5</v>
@@ -370,7 +370,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="n">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="B7" s="2" t="n">
         <v>6</v>
@@ -402,7 +402,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="n">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="B8" s="2" t="n">
         <v>7</v>
@@ -434,7 +434,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="n">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="B9" s="2" t="n">
         <v>8</v>
@@ -466,7 +466,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="n">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="B10" s="2" t="n">
         <v>9</v>
@@ -498,7 +498,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="n">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="B11" s="2" t="n">
         <v>10</v>
@@ -530,7 +530,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="n">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="B12" s="2" t="n">
         <v>11</v>
@@ -562,7 +562,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="n">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="B13" s="2" t="n">
         <v>12</v>
@@ -594,7 +594,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="n">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="B14" s="2" t="n">
         <v>13</v>
@@ -626,7 +626,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="n">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="B15" s="2" t="n">
         <v>14</v>
@@ -658,7 +658,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="n">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="B16" s="2" t="n">
         <v>15</v>
@@ -690,7 +690,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="n">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="B17" s="2" t="n">
         <v>16</v>

</xml_diff>